<commit_message>
Fix affichage mapping posologie e41663fffce190114f776fec6ae70ecf18a6d6aa
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
+++ b/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-26T15:31:22+00:00</t>
+    <t>2024-12-26T15:51:21+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -141,7 +141,7 @@
     <t>equivalent</t>
   </si>
   <si>
-    <t>Dosage.timing.repeat.periodUnit</t>
+    <t>Dosage.timing.repeat</t>
   </si>
   <si>
     <t>Elément_posologie/Fréquence_structurée/Frq_durée</t>

</xml_diff>

<commit_message>
Fix 2 affichage mapping Posologie b240e37fa0b9e3fc68e628cd0a724dccc7e76598
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
+++ b/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-27T09:52:33+00:00</t>
+    <t>2024-12-27T10:08:00+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -141,7 +141,7 @@
     <t>equivalent</t>
   </si>
   <si>
-    <t>Dosage.timing.repeat</t>
+    <t>Dosage.timing.repeat.periodUnit</t>
   </si>
   <si>
     <t>Elément_posologie/Fréquence_structurée/Frq_durée</t>

</xml_diff>

<commit_message>
Fix final affichage mapping posologie 5caaf5b998d9ab951bfcdc2d931a38eab5fcecf9
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
+++ b/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="52">
   <si>
     <t>Property</t>
   </si>
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-27T10:08:00+00:00</t>
+    <t>2024-12-27T10:41:44+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -635,9 +635,7 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="2">
-        <v>38</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
         <v>39</v>
@@ -648,9 +646,7 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>38</v>
-      </c>
+      <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>39</v>
@@ -661,9 +657,7 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="2">
-        <v>38</v>
-      </c>
+      <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
         <v>39</v>
@@ -674,9 +668,7 @@
       <c r="E6" s="2"/>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="2">
-        <v>38</v>
-      </c>
+      <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
         <v>39</v>
@@ -687,9 +679,7 @@
       <c r="E7" s="2"/>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="2">
-        <v>38</v>
-      </c>
+      <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
         <v>39</v>
@@ -700,9 +690,7 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="2">
-        <v>38</v>
-      </c>
+      <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
         <v>39</v>

</xml_diff>

<commit_message>
Essai fix non affichage comment 0ea57bfb4b2be47fc4db7e7a0f5ae2748fc099e0
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
+++ b/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="84">
   <si>
     <t>Property</t>
   </si>
@@ -126,7 +126,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-02T08:06:50+00:00</t>
+    <t>2025-01-02T08:36:24+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -286,6 +286,12 @@
   </si>
   <si>
     <t>Elément_posologie/Evt_structuré_début/Evénement_structuré/Evt_objet/Evt_période_nommée</t>
+  </si>
+  <si>
+    <t>Elément_posologie/Evt_structuré_début/Evénement_structuré/Evt_objet/Evt_clinique</t>
+  </si>
+  <si>
+    <t>not-related-to</t>
   </si>
   <si>
     <t>Elément_posologie/Durée/Nombre</t>
@@ -4369,6 +4375,60 @@
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4410,7 +4470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4453,7 +4513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4496,7 +4556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4539,7 +4599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4582,49 +4642,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E5"/>
@@ -4665,40 +4682,40 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>71</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
         <v>39</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>39</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -4803,40 +4820,40 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>75</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
         <v>39</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -4885,40 +4902,40 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>80</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
         <v>39</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E5" s="2"/>
     </row>

</xml_diff>

<commit_message>
Fix affichage comment d4a0f81e6045963d2498c29096cf3ccee8573c2c
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
+++ b/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="88">
   <si>
     <t>Property</t>
   </si>
@@ -126,7 +126,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-02T08:36:24+00:00</t>
+    <t>2025-01-02T08:46:33+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -292,6 +292,18 @@
   </si>
   <si>
     <t>not-related-to</t>
+  </si>
+  <si>
+    <t>Elément_posologie/Evt_structuré_début/Evénement_structuré</t>
+  </si>
+  <si>
+    <t>Elément_posologie/Type_événement2_début</t>
+  </si>
+  <si>
+    <t>Elément_posologie/Type_événement_fin</t>
+  </si>
+  <si>
+    <t>Elément_posologie/Type_événement2_fin</t>
   </si>
   <si>
     <t>Elément_posologie/Durée/Nombre</t>
@@ -4429,41 +4441,52 @@
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -4472,41 +4495,52 @@
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -4515,41 +4549,52 @@
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -4558,41 +4603,52 @@
 
 <file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -4601,41 +4657,52 @@
 
 <file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -4643,144 +4710,6 @@
 </file>
 
 <file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -4850,93 +4779,231 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="D5" t="s" s="2">
+      <c r="D3" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="E5" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s" s="2">
         <v>79</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>80</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
         <v>39</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>32</v>
       </c>
       <c r="D5" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2"/>
+      <c r="B2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" t="s" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
         <v>83</v>
       </c>
+      <c r="B3" s="2"/>
+      <c r="C3" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>87</v>
+      </c>
       <c r="E5" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix concept map aa706223046fb2ec39983cbc0fafe2b15e487067
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
+++ b/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="99">
   <si>
     <t>Property</t>
   </si>
@@ -132,7 +132,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-11T07:36:18+00:00</t>
+    <t>2025-04-12T14:29:05+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -5747,7 +5747,7 @@
 
 <file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5841,10 +5841,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -5854,10 +5854,10 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -5880,10 +5880,10 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -5893,10 +5893,10 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -5919,25 +5919,12 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E13" s="2"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="D14" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="E14" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Debut explication quantite composant prescrite d655a14d6da33e19e22d852bfe6e54ae433ef148
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
+++ b/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="99">
   <si>
     <t>Property</t>
   </si>
@@ -132,7 +132,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-12T14:29:05+00:00</t>
+    <t>2025-04-14T11:52:10+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -5254,7 +5254,7 @@
 
 <file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5296,7 +5296,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s" s="2">
         <v>81</v>
@@ -5312,7 +5312,7 @@
         <v>39</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -5351,7 +5351,7 @@
         <v>39</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -5364,7 +5364,7 @@
         <v>39</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -5377,9 +5377,22 @@
         <v>39</v>
       </c>
       <c r="D9" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Finalisation explication quantite composant prescrite f479c92e70054595ad2a6a1aeafe5edcc3604c4d
</commit_message>
<xml_diff>
--- a/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
+++ b/FinalisationMappingPosologie/ig/PN13-FHIR-prescmed-dosageinstruction-conceptmap.xlsx
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="99">
   <si>
     <t>Property</t>
   </si>
@@ -132,7 +132,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-04-14T11:52:10+00:00</t>
+    <t>2025-04-14T12:50:20+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -5522,7 +5522,7 @@
 
 <file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5564,7 +5564,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s" s="2">
         <v>86</v>
@@ -5590,10 +5590,10 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -5603,10 +5603,10 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -5645,7 +5645,7 @@
         <v>39</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="E9" s="2"/>
     </row>
@@ -5668,10 +5668,10 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -5681,10 +5681,10 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E12" s="2"/>
     </row>
@@ -5707,10 +5707,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" s="2"/>
     </row>
@@ -5720,10 +5720,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -5746,12 +5746,25 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="D17" t="s" s="2">
+      <c r="D18" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E18" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -5946,7 +5959,7 @@
 
 <file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5988,7 +6001,7 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s" s="2">
         <v>95</v>
@@ -6001,9 +6014,11 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>95</v>
+      </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
@@ -6019,15 +6034,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>97</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7">
@@ -6039,9 +6052,35 @@
         <v>32</v>
       </c>
       <c r="D7" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>